<commit_message>
Issue #12 + other docco
</commit_message>
<xml_diff>
--- a/templates/VocExcel-template-080-GA.xlsx
+++ b/templates/VocExcel-template-080-GA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/work/kurrawong/VocExcel/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFD8078-48E7-FA4F-9A57-C5E8DA196FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E21D1D-D899-3F43-A9A7-0044A3330D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="700" windowWidth="56960" windowHeight="28040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46740" yWindow="500" windowWidth="40920" windowHeight="27380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="183">
   <si>
     <t>Version:</t>
   </si>
@@ -916,25 +916,6 @@
   <si>
     <t>Classification of this vocab according to other vocabs or simple keywords.
 Separate multiple IRIs or keywords with commas</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial (Body)"/>
-      </rPr>
-      <t>Catalogue PID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial (Body)"/>
-      </rPr>
-      <t xml:space="preserve"> = A persistent identifier for this vocabulary in your catalogue system. Could be an IRI, a DOI or a numerical or textual ID, if this vocab has one</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1537,6 +1518,121 @@
   </si>
   <si>
     <t>A textual ID for this Concept. Must be letters and numbers and simple punctuation like full stop only.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Definition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>* = The definition of the Concept. Plain text only but paragraphs may be separated by newlines</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Definition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>* = The definition of the vocabulary. Plain text only but paragraphs may be separated by newlines</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve">eCat ID </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>= The persistent identifier for this vocabulary in the eCat catalogue system.
+Starting https://pid.geoscience.gov.au/dataset/…</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> = An example of this Concept. Plain text only, which may be prose or RDF data, able to be separated into paragraphs.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Image URL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> = a URL to an image that is avaiable online</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t>Image Embedded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> = A small - a few KB - image to be embedeed in the vocab for this Concept. Add the image file to the Cell: Insert &gt; Pictures &gt;Place in Cell &gt; Picture from File…</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2359,7 +2455,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
@@ -2370,7 +2466,7 @@
     <row r="5" spans="1:11" ht="57" x14ac:dyDescent="0.15">
       <c r="A5" s="59"/>
       <c r="B5" s="60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="59"/>
@@ -2400,7 +2496,7 @@
     <row r="7" spans="1:11" ht="19" x14ac:dyDescent="0.15">
       <c r="A7" s="59"/>
       <c r="B7" s="60" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="59"/>
       <c r="D7" s="59"/>
@@ -2414,7 +2510,7 @@
     <row r="8" spans="1:11" ht="19" x14ac:dyDescent="0.15">
       <c r="A8" s="59"/>
       <c r="B8" s="62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" s="59"/>
       <c r="D8" s="60" t="s">
@@ -2445,7 +2541,7 @@
     <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.15">
       <c r="A10" s="59"/>
       <c r="B10" s="60" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" s="59"/>
       <c r="D10" s="60"/>
@@ -2459,7 +2555,7 @@
     <row r="11" spans="1:11" ht="19" x14ac:dyDescent="0.15">
       <c r="A11" s="59"/>
       <c r="B11" s="62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C11" s="59"/>
       <c r="D11" s="60"/>
@@ -2485,7 +2581,7 @@
     <row r="13" spans="1:11" ht="41" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="59"/>
       <c r="B13" s="60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C13" s="59"/>
       <c r="D13" s="56"/>
@@ -2499,7 +2595,7 @@
     <row r="14" spans="1:11" ht="19" x14ac:dyDescent="0.15">
       <c r="A14" s="59"/>
       <c r="B14" s="62" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="59"/>
@@ -3593,10 +3689,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E056D66-684B-EA44-9D39-98A26FD38952}">
-  <dimension ref="A2:C64"/>
+  <dimension ref="A2:C68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="20" x14ac:dyDescent="0.15"/>
@@ -3748,88 +3844,88 @@
     <row r="24" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="16"/>
       <c r="B24" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="16"/>
       <c r="B25" s="7" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="16"/>
       <c r="B26" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="16"/>
       <c r="B27" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="16"/>
       <c r="B28" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="16"/>
       <c r="B29" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="16"/>
       <c r="B30" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="16"/>
       <c r="B31" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="49" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="16"/>
       <c r="B32" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="37" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="16"/>
       <c r="B33" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="16"/>
       <c r="B34" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="16"/>
       <c r="B35" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="50" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="38" x14ac:dyDescent="0.15">
       <c r="B38" s="7" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
@@ -3845,124 +3941,144 @@
     </row>
     <row r="41" spans="1:2" ht="46" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="7" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="46" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="52" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="38" x14ac:dyDescent="0.15">
       <c r="B47" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B48" s="7"/>
-    </row>
-    <row r="49" spans="1:2" ht="86" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="49" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B49" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B50" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="38" x14ac:dyDescent="0.15">
+      <c r="B51" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B52" s="7"/>
+    </row>
+    <row r="53" spans="1:2" ht="86" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B53" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="88" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B50" s="7" t="s">
+    <row r="54" spans="1:2" ht="88" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B54" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="7" t="s">
+    <row r="55" spans="1:2" ht="108" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B55" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="72" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="7" t="s">
+    <row r="56" spans="1:2" ht="72" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="57" x14ac:dyDescent="0.15">
-      <c r="B53" s="7" t="s">
+    <row r="57" spans="1:2" ht="57" x14ac:dyDescent="0.15">
+      <c r="B57" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="38" x14ac:dyDescent="0.15">
-      <c r="B54" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="38" x14ac:dyDescent="0.15">
-      <c r="B55" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B56" s="7"/>
-    </row>
-    <row r="57" spans="1:2" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="14" t="s">
+    <row r="58" spans="1:2" ht="38" x14ac:dyDescent="0.15">
+      <c r="B58" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="38" x14ac:dyDescent="0.15">
+      <c r="B59" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="1:2" ht="29" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B58" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B59" s="7" t="s">
+      <c r="B61" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B60" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="B61" s="7"/>
-    </row>
-    <row r="62" spans="1:2" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="14" t="s">
-        <v>31</v>
-      </c>
+    <row r="62" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="47" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B63" s="7" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B64" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B65" s="7"/>
+    </row>
+    <row r="66" spans="1:2" ht="47" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B67" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B68" s="7" t="s">
         <v>112</v>
       </c>
     </row>
@@ -3983,7 +4099,7 @@
   <dimension ref="A1:D1001"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4082,7 +4198,7 @@
       </c>
       <c r="B8" s="54"/>
       <c r="C8" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" s="33" t="s">
         <v>24</v>
@@ -4094,7 +4210,7 @@
       </c>
       <c r="B9" s="51"/>
       <c r="C9" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D9" s="33" t="s">
         <v>24</v>
@@ -4106,7 +4222,7 @@
       </c>
       <c r="B10" s="51"/>
       <c r="C10" s="33" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D10" s="33" t="s">
         <v>25</v>
@@ -4118,7 +4234,7 @@
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>11</v>
@@ -4130,7 +4246,7 @@
       </c>
       <c r="B12" s="53"/>
       <c r="C12" s="33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>3</v>
@@ -4145,7 +4261,7 @@
         <v>86</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="40" customHeight="1" x14ac:dyDescent="0.15">
@@ -4154,7 +4270,7 @@
       </c>
       <c r="B14" s="55"/>
       <c r="C14" s="33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" s="33" t="s">
         <v>93</v>
@@ -4166,7 +4282,7 @@
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>94</v>
@@ -4190,7 +4306,7 @@
       </c>
       <c r="B17" s="54"/>
       <c r="C17" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>83</v>
@@ -4198,14 +4314,14 @@
     </row>
     <row r="18" spans="1:4" ht="38" x14ac:dyDescent="0.15">
       <c r="A18" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" s="55"/>
       <c r="C18" s="33" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
@@ -7183,9 +7299,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B2936F-06B6-364A-893D-D48542B6FA7F}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0.15"/>
@@ -7244,13 +7360,13 @@
         <v>71</v>
       </c>
       <c r="J2" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="K2" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="K2" s="31" t="s">
+      <c r="L2" s="31" t="s">
         <v>169</v>
-      </c>
-      <c r="L2" s="31" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="271" customHeight="1" x14ac:dyDescent="0.15">
@@ -7258,37 +7374,37 @@
         <v>87</v>
       </c>
       <c r="B3" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>129</v>
-      </c>
       <c r="D3" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>47</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>86</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I3" s="60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J3" s="60" t="s">
+        <v>170</v>
+      </c>
+      <c r="K3" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="K3" s="60" t="s">
+      <c r="L3" s="60" t="s">
         <v>172</v>
-      </c>
-      <c r="L3" s="60" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
@@ -7638,7 +7754,7 @@
         <v>63</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:27" s="20" customFormat="1" ht="266" x14ac:dyDescent="0.15">
@@ -7651,10 +7767,10 @@
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
       <c r="G3" s="46" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
@@ -7770,16 +7886,16 @@
     <row r="3" spans="1:7" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" s="63"/>
       <c r="B3" s="64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C3" s="64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D3" s="64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E3" s="64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="20" customFormat="1" ht="18" x14ac:dyDescent="0.15">
@@ -9305,6 +9421,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006CE8352A0AF1CD4AB9B3521FB05BB06E" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad776eddaa4c2424eb5fa9eef7239753">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcd33c6e-30cb-4633-b8ec-d716de95c77b" xmlns:ns3="cc9fd5b5-cf46-4eda-9201-7118bc1c1603" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c03cb13ad1de5dce1c8a6420670aeaf6" ns2:_="" ns3:_="">
     <xsd:import namespace="bcd33c6e-30cb-4633-b8ec-d716de95c77b"/>
@@ -9541,16 +9666,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C0741D-72E1-4141-9700-3202E4B56A5A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35C5B03A-DD20-4DDE-9069-342AD74757E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9567,12 +9691,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41C0741D-72E1-4141-9700-3202E4B56A5A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>